<commit_message>
Cleaner Directories - Added 3Applications for testing and growth curve
</commit_message>
<xml_diff>
--- a/multi_growth_app/active_runs/Sample Excel Experiment Run Document (copy).xlsx
+++ b/multi_growth_app/active_runs/Sample Excel Experiment Run Document (copy).xlsx
@@ -146,8 +146,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,7 +183,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -214,19 +218,19 @@
         <f aca="false">IF((COLUMN() -1) &lt;= $B$1, COLUMN() - 1, "")</f>
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="str">
+      <c r="D3" s="2" t="str">
         <f aca="false">IF((COLUMN() -1) &lt;= $B$1, COLUMN() - 1, "")</f>
         <v/>
       </c>
-      <c r="E3" s="1" t="str">
+      <c r="E3" s="2" t="str">
         <f aca="false">IF((COLUMN() -1) &lt;= $B$1, COLUMN() - 1, "")</f>
         <v/>
       </c>
-      <c r="F3" s="1" t="str">
+      <c r="F3" s="2" t="str">
         <f aca="false">IF((COLUMN() -1) &lt;= $B$1, COLUMN() - 1, "")</f>
         <v/>
       </c>
-      <c r="G3" s="1" t="str">
+      <c r="G3" s="2" t="str">
         <f aca="false">IF((COLUMN() -1) &lt;= $B$1, COLUMN() - 1, "")</f>
         <v/>
       </c>
@@ -259,45 +263,45 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="B4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -11069,401 +11073,401 @@
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11475,401 +11479,401 @@
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" s="0" t="n">
         <f aca="false">IF(OR(ISBLANK(Complete_Run_Layout!$C$4),ISBLANK(Complete_Run_Layout!$C$5),ISBLANK(Complete_Run_Layout!$C$3), Complete_Run_Layout!$C$3 = ""), "", Complete_Run_Layout!$C$5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>